<commit_message>
solved tanggal lahir on import data
</commit_message>
<xml_diff>
--- a/assets/import/file/test.xlsx
+++ b/assets/import/file/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\app-absen\assets\import\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD8B4B6-9217-4076-9535-DB919915B984}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B8D12-90A9-400F-B793-6F421665B928}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="795" windowWidth="15375" windowHeight="7995" xr2:uid="{B38DEA1A-B9F6-4C14-9912-15C8999A1FAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B38DEA1A-B9F6-4C14-9912-15C8999A1FAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
   <si>
     <t>NISN</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Test data 2</t>
   </si>
   <si>
-    <t>2021/2023</t>
-  </si>
-  <si>
     <t>Test tempat 2</t>
   </si>
   <si>
@@ -78,154 +75,100 @@
     <t>Test tempat 3</t>
   </si>
   <si>
-    <t>2021/2024</t>
-  </si>
-  <si>
     <t>Test data 4</t>
   </si>
   <si>
     <t>Test tempat 4</t>
   </si>
   <si>
-    <t>2021/2025</t>
-  </si>
-  <si>
     <t>Test tempat 5</t>
   </si>
   <si>
-    <t>2021/2026</t>
-  </si>
-  <si>
     <t>Test data 6</t>
   </si>
   <si>
     <t>Test tempat 6</t>
   </si>
   <si>
-    <t>2021/2027</t>
-  </si>
-  <si>
     <t>Test data 7</t>
   </si>
   <si>
     <t>Test tempat 7</t>
   </si>
   <si>
-    <t>2021/2028</t>
-  </si>
-  <si>
     <t>Test data 8</t>
   </si>
   <si>
     <t>Test tempat 8</t>
   </si>
   <si>
-    <t>2021/2029</t>
-  </si>
-  <si>
     <t>Test data 9</t>
   </si>
   <si>
     <t>Test tempat 9</t>
   </si>
   <si>
-    <t>2021/2030</t>
-  </si>
-  <si>
     <t>Test data 10</t>
   </si>
   <si>
     <t>Test tempat 10</t>
   </si>
   <si>
-    <t>2021/2031</t>
-  </si>
-  <si>
     <t>Test tempat 11</t>
   </si>
   <si>
-    <t>2021/2032</t>
-  </si>
-  <si>
     <t>Test data 12</t>
   </si>
   <si>
     <t>Test tempat 12</t>
   </si>
   <si>
-    <t>2021/2033</t>
-  </si>
-  <si>
     <t>Test data 13</t>
   </si>
   <si>
     <t>Test tempat 13</t>
   </si>
   <si>
-    <t>2021/2034</t>
-  </si>
-  <si>
     <t>Test data 14</t>
   </si>
   <si>
     <t>Test tempat 14</t>
   </si>
   <si>
-    <t>2021/2035</t>
-  </si>
-  <si>
     <t>Test data 15</t>
   </si>
   <si>
     <t>Test tempat 15</t>
   </si>
   <si>
-    <t>2021/2036</t>
-  </si>
-  <si>
     <t>Test data 16</t>
   </si>
   <si>
     <t>Test tempat 16</t>
   </si>
   <si>
-    <t>2021/2037</t>
-  </si>
-  <si>
     <t>Test data 17</t>
   </si>
   <si>
     <t>Test tempat 17</t>
   </si>
   <si>
-    <t>2021/2038</t>
-  </si>
-  <si>
     <t>Test data 18</t>
   </si>
   <si>
     <t>Test tempat 18</t>
   </si>
   <si>
-    <t>2021/2039</t>
-  </si>
-  <si>
     <t>Test data 19</t>
   </si>
   <si>
     <t>Test tempat 19</t>
   </si>
   <si>
-    <t>2021/2040</t>
-  </si>
-  <si>
     <t>Test data 20</t>
   </si>
   <si>
     <t>Test tempat 20</t>
-  </si>
-  <si>
-    <t>2021/2041</t>
   </si>
   <si>
     <t>Mulyadih</t>
@@ -601,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F1B7BC-923B-4F21-B9E7-6AED7C906DD6}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>43936</v>
@@ -670,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
         <v>43937</v>
@@ -682,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -690,10 +633,10 @@
         <v>99123123126</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>43938</v>
@@ -705,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,10 +656,10 @@
         <v>99123123127</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>43939</v>
@@ -728,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -736,10 +679,10 @@
         <v>99123123123</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2">
         <v>43940</v>
@@ -751,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -759,10 +702,10 @@
         <v>99123123129</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2">
         <v>43941</v>
@@ -774,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -782,10 +725,10 @@
         <v>99123123130</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2">
         <v>43942</v>
@@ -797,7 +740,7 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,10 +748,10 @@
         <v>99123123131</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2">
         <v>43943</v>
@@ -820,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -828,10 +771,10 @@
         <v>99123123132</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2">
         <v>43944</v>
@@ -843,15 +786,15 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>43945</v>
@@ -863,7 +806,7 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -871,10 +814,10 @@
         <v>99123123122</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2">
         <v>43946</v>
@@ -886,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -894,10 +837,10 @@
         <v>99123123135</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2">
         <v>43947</v>
@@ -909,7 +852,7 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,10 +860,10 @@
         <v>99123123136</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2">
         <v>43948</v>
@@ -932,7 +875,7 @@
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,10 +883,10 @@
         <v>99123123137</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2">
         <v>43949</v>
@@ -955,7 +898,7 @@
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -963,10 +906,10 @@
         <v>99123123138</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2">
         <v>43950</v>
@@ -978,7 +921,7 @@
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -986,10 +929,10 @@
         <v>99123123139</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2">
         <v>43951</v>
@@ -1001,7 +944,7 @@
         <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,10 +952,10 @@
         <v>99123123140</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2">
         <v>43952</v>
@@ -1024,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1032,10 +975,10 @@
         <v>99123123141</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
         <v>43953</v>
@@ -1047,7 +990,7 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1055,10 +998,10 @@
         <v>99123123142</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2">
         <v>43954</v>
@@ -1070,7 +1013,7 @@
         <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,10 +1021,10 @@
         <v>99123123143</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2">
         <v>43955</v>
@@ -1093,7 +1036,7 @@
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>